<commit_message>
Update partner slide with Michael Fortner's slides. Update project to have new location for certificate files.
</commit_message>
<xml_diff>
--- a/ww101-shield/Pinouts.xlsx
+++ b/ww101-shield/Pinouts.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18201"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="93">
   <si>
     <t>CYW943907AEVAL1F</t>
   </si>
@@ -312,11 +312,14 @@
   <si>
     <t>D19</t>
   </si>
+  <si>
+    <t>GPIO (unused)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -339,7 +342,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -481,7 +484,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -517,7 +520,11 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -611,6 +618,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -646,6 +670,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -825,14 +866,14 @@
   <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="39.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="27" bestFit="1" customWidth="1"/>
@@ -1069,7 +1110,7 @@
       </c>
       <c r="B11" s="2"/>
       <c r="C11" t="s">
-        <v>31</v>
+        <v>92</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>39</v>
@@ -1101,11 +1142,11 @@
       <c r="I12" s="2"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="22" t="s">
         <v>12</v>
       </c>
       <c r="B13" s="2"/>
-      <c r="C13" t="s">
+      <c r="C13" s="19" t="s">
         <v>28</v>
       </c>
       <c r="D13" s="1" t="s">
@@ -1122,13 +1163,13 @@
       <c r="I13" s="2"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="22" t="s">
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="19" t="s">
         <v>29</v>
       </c>
       <c r="D14" s="1" t="s">
@@ -1231,13 +1272,13 @@
       <c r="I19" s="2"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="22" t="s">
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C20" s="19" t="s">
+      <c r="C20" s="20" t="s">
         <v>27</v>
       </c>
       <c r="D20" s="1" t="s">
@@ -1256,11 +1297,11 @@
       <c r="I20" s="2"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+      <c r="A21" s="22" t="s">
         <v>20</v>
       </c>
       <c r="B21" s="2"/>
-      <c r="C21" s="19" t="s">
+      <c r="C21" s="20" t="s">
         <v>26</v>
       </c>
       <c r="D21" s="1" t="s">
@@ -1275,11 +1316,11 @@
       <c r="I21" s="2"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+      <c r="A22" s="22" t="s">
         <v>21</v>
       </c>
       <c r="B22" s="2"/>
-      <c r="C22" s="19" t="s">
+      <c r="C22" s="20" t="s">
         <v>30</v>
       </c>
       <c r="D22" s="1" t="s">
@@ -1294,13 +1335,13 @@
       <c r="I22" s="2"/>
     </row>
     <row r="23" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
+      <c r="A23" s="22" t="s">
         <v>90</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C23" s="5" t="s">
+      <c r="C23" s="20" t="s">
         <v>25</v>
       </c>
       <c r="D23" s="1" t="s">
@@ -1319,13 +1360,13 @@
       <c r="I23" s="2"/>
     </row>
     <row r="24" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="3" t="s">
+      <c r="A24" s="23" t="s">
         <v>91</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C24" s="6" t="s">
+      <c r="C24" s="21" t="s">
         <v>25</v>
       </c>
       <c r="D24" s="3" t="s">
@@ -1351,7 +1392,7 @@
     <mergeCell ref="A1:B1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Update projects for chapter 6
</commit_message>
<xml_diff>
--- a/ww101-shield/Pinouts.xlsx
+++ b/ww101-shield/Pinouts.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="93">
   <si>
     <t>CYW943907AEVAL1F</t>
   </si>
@@ -484,7 +484,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -507,7 +507,11 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -520,11 +524,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -863,10 +865,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I24"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="F3" sqref="F3:G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -878,32 +880,26 @@
     <col min="5" max="5" width="39.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="27" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="31.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.42578125" customWidth="1"/>
-    <col min="9" max="9" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="B1" s="18"/>
+      <c r="B1" s="22"/>
       <c r="C1" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="16"/>
-      <c r="F1" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="16"/>
-      <c r="H1" s="15" t="s">
+      <c r="E1" s="20"/>
+      <c r="F1" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="I1" s="16"/>
-    </row>
-    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G1" s="20"/>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>84</v>
       </c>
@@ -925,14 +921,8 @@
       <c r="G2" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="H2" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -946,16 +936,14 @@
       <c r="E3" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G3" s="24" t="s">
         <v>88</v>
       </c>
-      <c r="H3" s="1"/>
-      <c r="I3" s="2"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -969,12 +957,10 @@
       <c r="E4" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="F4" s="10"/>
+      <c r="F4" s="1"/>
       <c r="G4" s="7"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="2"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -988,10 +974,10 @@
       <c r="E5" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="H5" s="1"/>
-      <c r="I5" s="2"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F5" s="1"/>
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1003,12 +989,10 @@
       <c r="E6" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="F6" s="10"/>
+      <c r="F6" s="1"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="2"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -1022,16 +1006,14 @@
       <c r="E7" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="F7" s="1" t="s">
         <v>69</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="H7" s="1"/>
-      <c r="I7" s="2"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -1045,16 +1027,14 @@
       <c r="E8" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="F8" s="1" t="s">
         <v>68</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="H8" s="1"/>
-      <c r="I8" s="2"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -1070,16 +1050,14 @@
       <c r="E9" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F9" s="10" t="s">
+      <c r="F9" s="1" t="s">
         <v>78</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="H9" s="1"/>
-      <c r="I9" s="2"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -1095,16 +1073,14 @@
       <c r="E10" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F10" s="10" t="s">
+      <c r="F10" s="1" t="s">
         <v>79</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="H10" s="1"/>
-      <c r="I10" s="2"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -1116,16 +1092,14 @@
         <v>39</v>
       </c>
       <c r="E11" s="2"/>
-      <c r="F11" s="10" t="s">
+      <c r="F11" s="1" t="s">
         <v>73</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="H11" s="1"/>
-      <c r="I11" s="2"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -1138,38 +1112,36 @@
       <c r="E12" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="H12" s="1"/>
-      <c r="I12" s="2"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="22" t="s">
+      <c r="F12" s="1"/>
+      <c r="G12" s="2"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="17" t="s">
         <v>12</v>
       </c>
       <c r="B13" s="2"/>
-      <c r="C13" s="19" t="s">
+      <c r="C13" s="14" t="s">
         <v>28</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>41</v>
       </c>
       <c r="E13" s="2"/>
-      <c r="F13" s="10" t="s">
+      <c r="F13" s="1" t="s">
         <v>65</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="H13" s="1"/>
-      <c r="I13" s="2"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="22" t="s">
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="17" t="s">
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="19" t="s">
+      <c r="C14" s="14" t="s">
         <v>29</v>
       </c>
       <c r="D14" s="1" t="s">
@@ -1178,16 +1150,14 @@
       <c r="E14" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="F14" s="10" t="s">
+      <c r="F14" s="1" t="s">
         <v>63</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="H14" s="1"/>
-      <c r="I14" s="2"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
@@ -1200,10 +1170,10 @@
       <c r="E15" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="H15" s="1"/>
-      <c r="I15" s="2"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F15" s="1"/>
+      <c r="G15" s="2"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
@@ -1212,11 +1182,10 @@
         <v>43</v>
       </c>
       <c r="E16" s="2"/>
+      <c r="F16" s="1"/>
       <c r="G16" s="2"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="2"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
@@ -1226,12 +1195,10 @@
         <v>44</v>
       </c>
       <c r="E17" s="2"/>
-      <c r="F17" s="10"/>
+      <c r="F17" s="1"/>
       <c r="G17" s="2"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="2"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
@@ -1245,12 +1212,10 @@
       <c r="E18" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="F18" s="10"/>
+      <c r="F18" s="1"/>
       <c r="G18" s="2"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="2"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
@@ -1264,21 +1229,19 @@
       <c r="E19" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="F19" s="14" t="s">
+      <c r="F19" s="25" t="s">
         <v>87</v>
       </c>
       <c r="G19" s="2"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="2"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="22" t="s">
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="17" t="s">
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C20" s="20" t="s">
+      <c r="C20" s="15" t="s">
         <v>27</v>
       </c>
       <c r="D20" s="1" t="s">
@@ -1287,61 +1250,55 @@
       <c r="E20" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="F20" s="10" t="s">
+      <c r="F20" s="1" t="s">
         <v>62</v>
       </c>
       <c r="G20" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="H20" s="1"/>
-      <c r="I20" s="2"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="22" t="s">
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="17" t="s">
         <v>20</v>
       </c>
       <c r="B21" s="2"/>
-      <c r="C21" s="20" t="s">
+      <c r="C21" s="15" t="s">
         <v>26</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>48</v>
       </c>
       <c r="E21" s="2"/>
-      <c r="F21" s="10" t="s">
+      <c r="F21" s="1" t="s">
         <v>76</v>
       </c>
       <c r="G21" s="2"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="2"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="22" t="s">
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="17" t="s">
         <v>21</v>
       </c>
       <c r="B22" s="2"/>
-      <c r="C22" s="20" t="s">
+      <c r="C22" s="15" t="s">
         <v>30</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>49</v>
       </c>
       <c r="E22" s="2"/>
-      <c r="F22" s="10" t="s">
+      <c r="F22" s="1" t="s">
         <v>77</v>
       </c>
       <c r="G22" s="2"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="2"/>
-    </row>
-    <row r="23" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="22" t="s">
+    </row>
+    <row r="23" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="17" t="s">
         <v>90</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C23" s="20" t="s">
+      <c r="C23" s="15" t="s">
         <v>25</v>
       </c>
       <c r="D23" s="1" t="s">
@@ -1350,23 +1307,21 @@
       <c r="E23" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="F23" s="10" t="s">
+      <c r="F23" s="1" t="s">
         <v>69</v>
       </c>
       <c r="G23" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="H23" s="1"/>
-      <c r="I23" s="2"/>
-    </row>
-    <row r="24" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="23" t="s">
+    </row>
+    <row r="24" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="18" t="s">
         <v>91</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C24" s="21" t="s">
+      <c r="C24" s="16" t="s">
         <v>25</v>
       </c>
       <c r="D24" s="3" t="s">
@@ -1375,18 +1330,15 @@
       <c r="E24" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="F24" s="11" t="s">
+      <c r="F24" s="3" t="s">
         <v>68</v>
       </c>
       <c r="G24" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="H24" s="3"/>
-      <c r="I24" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="H1:I1"/>
+  <mergeCells count="3">
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="A1:B1"/>
@@ -1418,25 +1370,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="B1" s="18"/>
+      <c r="B1" s="22"/>
       <c r="C1" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="16"/>
-      <c r="F1" s="15" t="s">
+      <c r="E1" s="20"/>
+      <c r="F1" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="16"/>
-      <c r="H1" s="15" t="s">
+      <c r="G1" s="20"/>
+      <c r="H1" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="I1" s="16"/>
+      <c r="I1" s="20"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">

</xml_diff>

<commit_message>
Update manual for 07b as AWS, 07c as HTTP, and 07d as MQTT. Also affects the signoff sheet, intro (agenda) and class project. The revision on the binder is now 2.1.
</commit_message>
<xml_diff>
--- a/ww101-shield/Pinouts.xlsx
+++ b/ww101-shield/Pinouts.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="95">
   <si>
     <t>CYW943907AEVAL1F</t>
   </si>
@@ -314,6 +314,12 @@
   </si>
   <si>
     <t>GPIO (unused)</t>
+  </si>
+  <si>
+    <t>MB2</t>
+  </si>
+  <si>
+    <t>LED2</t>
   </si>
 </sst>
 </file>
@@ -512,6 +518,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -524,9 +533,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -868,7 +874,7 @@
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3:G24"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -883,21 +889,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="24" t="s">
         <v>82</v>
       </c>
-      <c r="B1" s="22"/>
+      <c r="B1" s="25"/>
       <c r="C1" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="20"/>
-      <c r="F1" s="19" t="s">
+      <c r="E1" s="23"/>
+      <c r="F1" s="22" t="s">
         <v>89</v>
       </c>
-      <c r="G1" s="20"/>
+      <c r="G1" s="23"/>
     </row>
     <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
@@ -936,10 +942,10 @@
       <c r="E3" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="F3" s="23" t="s">
+      <c r="F3" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="G3" s="24" t="s">
+      <c r="G3" s="20" t="s">
         <v>88</v>
       </c>
     </row>
@@ -1229,7 +1235,7 @@
       <c r="E19" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="F19" s="25" t="s">
+      <c r="F19" s="21" t="s">
         <v>87</v>
       </c>
       <c r="G19" s="2"/>
@@ -1242,7 +1248,7 @@
         <v>24</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>27</v>
+        <v>94</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>47</v>
@@ -1263,7 +1269,7 @@
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="15" t="s">
-        <v>26</v>
+        <v>93</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>48</v>
@@ -1370,25 +1376,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="24" t="s">
         <v>82</v>
       </c>
-      <c r="B1" s="22"/>
+      <c r="B1" s="25"/>
       <c r="C1" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="20"/>
-      <c r="F1" s="19" t="s">
+      <c r="E1" s="23"/>
+      <c r="F1" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="20"/>
-      <c r="H1" s="19" t="s">
+      <c r="G1" s="23"/>
+      <c r="H1" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="I1" s="20"/>
+      <c r="I1" s="23"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">

</xml_diff>